<commit_message>
kWh/m should be m/kWh
</commit_message>
<xml_diff>
--- a/ICE v BEV.xlsx
+++ b/ICE v BEV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a113766d58a748/Personal/CAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{F204D04E-0357-4B2A-9E1C-6CF952B1BCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE25939F-C179-459E-B6E0-2DB6D4F5D0BA}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{F204D04E-0357-4B2A-9E1C-6CF952B1BCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB245B31-287D-4C85-A890-C3A6F84AAC94}"/>
   <bookViews>
-    <workbookView xWindow="-26400" yWindow="795" windowWidth="23970" windowHeight="13290" xr2:uid="{914A0BA3-2E55-48BC-A3AF-8D79FC10525F}"/>
+    <workbookView xWindow="-24975" yWindow="1965" windowWidth="23970" windowHeight="13290" activeTab="1" xr2:uid="{914A0BA3-2E55-48BC-A3AF-8D79FC10525F}"/>
   </bookViews>
   <sheets>
     <sheet name="ICE v BEV" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>efficiency mpg</t>
   </si>
   <si>
-    <t>efficiency kWh/m</t>
-  </si>
-  <si>
     <t>Measure</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>EV6</t>
+  </si>
+  <si>
+    <t>efficiency m/kWh</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416ADE44-C0D8-404F-A696-BA7CC4522A48}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,16 +626,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -682,7 +682,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="4">
@@ -692,14 +692,14 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1">
         <v>4.4000000000000004</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
         <f>(C10*(D10/100))+(C11*(D11/100))+(C12*(D12/100))</f>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFDB2EF-F7DD-4D40-9111-D303714F9FC2}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,42 +806,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -858,11 +858,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -879,11 +879,11 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -900,11 +900,11 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -921,11 +921,11 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -942,11 +942,11 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -963,11 +963,11 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -984,16 +984,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>2020</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1">
         <v>64</v>
@@ -1014,16 +1014,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
         <v>2021</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1">
         <v>77.400000000000006</v>
@@ -1044,13 +1044,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
         <v>2011</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>2016</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1090,11 +1090,11 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1108,11 +1108,11 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1129,11 +1129,11 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1147,11 +1147,11 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1165,11 +1165,11 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1183,11 +1183,11 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1201,11 +1201,11 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1219,11 +1219,11 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1237,11 +1237,11 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1255,11 +1255,11 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>

</xml_diff>